<commit_message>
Updated the scripts for riskperception dataset reading
</commit_message>
<xml_diff>
--- a/Datasets/housinggame_session_20_251007_surveys/251009_251007_WhereWeMove sessions - presurvey.xlsx
+++ b/Datasets/housinggame_session_20_251007_surveys/251009_251007_WhereWeMove sessions - presurvey.xlsx
@@ -5,21 +5,33 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/jcortesarevalo_tudelft_nl/Documents/Documents/TUDelft/18_Game Data Analysis/R data analysis BEPs/Datasets/housinggame_session_20_251007_VerzekeraarsMasterClass_surveys/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/jcortesarevalo_tudelft_nl/Documents/Documents/TUDelft/18_Game Data Analysis/R data analysis BEPs/Datasets/housinggame_session_20_251007_surveys/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_F267ED7BEE40FE1B69EAED488EA404700F25161E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94D372DB-EDE7-40AE-B804-5D89E6E43AC8}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_F267ED7BEE40FE1B69EAED488EA404700F25161E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C8D3BA4-1F6E-434F-93BC-B0ABC52D9E03}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet0!$A$2:$AH$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet0!$A$3:$AH$27</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -897,127 +909,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH25"/>
+  <dimension ref="A1:AH26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection sqref="A1:AH1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+      <c r="R1">
+        <v>18</v>
+      </c>
+      <c r="S1">
+        <v>19</v>
+      </c>
+      <c r="T1">
+        <v>20</v>
+      </c>
+      <c r="U1">
+        <v>21</v>
+      </c>
+      <c r="V1">
+        <v>22</v>
+      </c>
+      <c r="W1">
+        <v>23</v>
+      </c>
+      <c r="X1">
+        <v>24</v>
+      </c>
+      <c r="Y1">
+        <v>25</v>
+      </c>
+      <c r="Z1">
+        <v>26</v>
+      </c>
+      <c r="AA1">
+        <v>27</v>
+      </c>
+      <c r="AB1">
+        <v>28</v>
+      </c>
+      <c r="AC1">
+        <v>29</v>
+      </c>
+      <c r="AD1">
+        <v>30</v>
+      </c>
+      <c r="AE1">
+        <v>31</v>
+      </c>
+      <c r="AF1">
+        <v>32</v>
+      </c>
+      <c r="AG1">
+        <v>33</v>
+      </c>
+      <c r="AH1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -1029,218 +1041,218 @@
         <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="195" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="4" spans="1:34" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>45937.245208333334</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>45937.248240740744</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>261</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="1">
-        <v>45937.248254502316</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" ht="240" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>45937.248032407406</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45937.250648148147</v>
       </c>
       <c r="C4">
         <v>100</v>
       </c>
       <c r="D4">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F4" s="1">
-        <v>45937.250662881946</v>
+        <v>45937.248254502316</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>66</v>
@@ -1249,13 +1261,13 @@
         <v>67</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>70</v>
@@ -1264,46 +1276,46 @@
         <v>71</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>85</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>88</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="Z4" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="AC4" s="2" t="s">
         <v>77</v>
@@ -1312,39 +1324,39 @@
         <v>77</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AF4" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="180" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>45937.248437499999</v>
+        <v>45937.248032407406</v>
       </c>
       <c r="B5" s="1">
-        <v>45937.250694444447</v>
+        <v>45937.250648148147</v>
       </c>
       <c r="C5">
         <v>100</v>
       </c>
       <c r="D5">
-        <v>194</v>
+        <v>226</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="1">
-        <v>45937.250705486113</v>
+        <v>45937.250662881946</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>66</v>
@@ -1356,10 +1368,10 @@
         <v>68</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>70</v>
@@ -1368,87 +1380,87 @@
         <v>71</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="S5" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="AC5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AD5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AG5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>78</v>
-      </c>
     </row>
-    <row r="6" spans="1:34" ht="195" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="174" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>45937.24800925926</v>
+        <v>45937.248437499999</v>
       </c>
       <c r="B6" s="1">
-        <v>45937.250706018516</v>
+        <v>45937.250694444447</v>
       </c>
       <c r="C6">
         <v>100</v>
       </c>
       <c r="D6">
-        <v>232</v>
+        <v>194</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F6" s="1">
-        <v>45937.250719328702</v>
+        <v>45937.250705486113</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>66</v>
@@ -1460,61 +1472,61 @@
         <v>68</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AD6" s="2" t="s">
         <v>96</v>
@@ -1523,36 +1535,36 @@
         <v>77</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>45937.248159722221</v>
+        <v>45937.24800925926</v>
       </c>
       <c r="B7" s="1">
-        <v>45937.250810185185</v>
+        <v>45937.250706018516</v>
       </c>
       <c r="C7">
         <v>100</v>
       </c>
       <c r="D7">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F7" s="1">
-        <v>45937.250817812499</v>
+        <v>45937.250719328702</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>66</v>
@@ -1564,55 +1576,55 @@
         <v>68</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="T7" s="2" t="s">
         <v>72</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="V7" s="2" t="s">
         <v>73</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB7" s="2" t="s">
         <v>79</v>
@@ -1630,33 +1642,33 @@
         <v>77</v>
       </c>
       <c r="AG7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH7" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>45937.248622685183</v>
+        <v>45937.248159722221</v>
       </c>
       <c r="B8" s="1">
-        <v>45937.250821759262</v>
+        <v>45937.250810185185</v>
       </c>
       <c r="C8">
         <v>100</v>
       </c>
       <c r="D8">
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F8" s="1">
-        <v>45937.250835729166</v>
+        <v>45937.250817812499</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>66</v>
@@ -1668,99 +1680,99 @@
         <v>68</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="P8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="Q8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="V8" s="2" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="W8" s="2" t="s">
         <v>88</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="Y8" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="AA8" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AB8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD8" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AC8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AE8" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AF8" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AG8" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AH8" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>45937.247939814813</v>
+        <v>45937.248622685183</v>
       </c>
       <c r="B9" s="1">
-        <v>45937.251446759263</v>
+        <v>45937.250821759262</v>
       </c>
       <c r="C9">
         <v>100</v>
       </c>
       <c r="D9">
-        <v>303</v>
+        <v>190</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F9" s="1">
-        <v>45937.251459236111</v>
+        <v>45937.250835729166</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>66</v>
@@ -1772,99 +1784,99 @@
         <v>68</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>85</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="Y9" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA9" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AE9" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AF9" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AG9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH9" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="180" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>45937.248333333337</v>
+        <v>45937.247939814813</v>
       </c>
       <c r="B10" s="1">
-        <v>45937.251562500001</v>
+        <v>45937.251446759263</v>
       </c>
       <c r="C10">
         <v>100</v>
       </c>
       <c r="D10">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F10" s="1">
-        <v>45937.251572372683</v>
+        <v>45937.251459236111</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>66</v>
@@ -1876,99 +1888,99 @@
         <v>68</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>92</v>
       </c>
       <c r="P10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="Q10" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="R10" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AB10" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="AE10" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AH10" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="174" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>45937.247997685183</v>
+        <v>45937.248333333337</v>
       </c>
       <c r="B11" s="1">
-        <v>45937.251967592594</v>
+        <v>45937.251562500001</v>
       </c>
       <c r="C11">
         <v>100</v>
       </c>
       <c r="D11">
-        <v>343</v>
+        <v>279</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F11" s="1">
-        <v>45937.251981296293</v>
+        <v>45937.251572372683</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>66</v>
@@ -1980,64 +1992,64 @@
         <v>68</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>70</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>123</v>
+        <v>71</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="P11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="Q11" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="R11" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="S11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="T11" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="U11" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="W11" s="2" t="s">
         <v>88</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="Z11" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AC11" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="AE11" s="2" t="s">
         <v>77</v>
@@ -2052,27 +2064,27 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>45937.248333333337</v>
+        <v>45937.247997685183</v>
       </c>
       <c r="B12" s="1">
-        <v>45937.252164351848</v>
+        <v>45937.251967592594</v>
       </c>
       <c r="C12">
         <v>100</v>
       </c>
       <c r="D12">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F12" s="1">
-        <v>45937.252174247682</v>
+        <v>45937.251981296293</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>66</v>
@@ -2084,43 +2096,43 @@
         <v>68</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>83</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="U12" s="2" t="s">
         <v>85</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="X12" s="2" t="s">
         <v>124</v>
@@ -2129,10 +2141,10 @@
         <v>95</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AB12" s="2" t="s">
         <v>96</v>
@@ -2141,42 +2153,42 @@
         <v>77</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AE12" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AG12" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>45937.245358796295</v>
+        <v>45937.248333333337</v>
       </c>
       <c r="B13" s="1">
-        <v>45937.252199074072</v>
+        <v>45937.252164351848</v>
       </c>
       <c r="C13">
         <v>100</v>
       </c>
       <c r="D13">
-        <v>590</v>
+        <v>330</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F13" s="1">
-        <v>45937.252205034725</v>
+        <v>45937.252174247682</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>66</v>
@@ -2188,55 +2200,55 @@
         <v>68</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>83</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="U13" s="2" t="s">
         <v>85</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="Y13" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB13" s="2" t="s">
         <v>96</v>
@@ -2245,42 +2257,42 @@
         <v>77</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AE13" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AF13" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AG13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AH13" s="2" t="s">
-        <v>109</v>
-      </c>
     </row>
-    <row r="14" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>45937.249571759261</v>
+        <v>45937.245358796295</v>
       </c>
       <c r="B14" s="1">
-        <v>45937.252314814818</v>
+        <v>45937.252199074072</v>
       </c>
       <c r="C14">
         <v>100</v>
       </c>
       <c r="D14">
-        <v>236</v>
+        <v>590</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F14" s="1">
-        <v>45937.252322499997</v>
+        <v>45937.252205034725</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>66</v>
@@ -2292,22 +2304,22 @@
         <v>68</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>71</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>72</v>
@@ -2316,13 +2328,13 @@
         <v>83</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="T14" s="2" t="s">
         <v>72</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="V14" s="2" t="s">
         <v>73</v>
@@ -2337,54 +2349,54 @@
         <v>95</v>
       </c>
       <c r="Z14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH14" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AA14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG14" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH14" s="2" t="s">
-        <v>79</v>
-      </c>
     </row>
-    <row r="15" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>45937.249456018515</v>
+        <v>45937.249571759261</v>
       </c>
       <c r="B15" s="1">
-        <v>45937.25236111111</v>
+        <v>45937.252314814818</v>
       </c>
       <c r="C15">
         <v>100</v>
       </c>
       <c r="D15">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F15" s="1">
-        <v>45937.252370150462</v>
+        <v>45937.252322499997</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>66</v>
@@ -2396,43 +2408,43 @@
         <v>68</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="O15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="P15" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="S15" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="V15" s="2" t="s">
         <v>73</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="X15" s="2" t="s">
         <v>94</v>
@@ -2441,7 +2453,7 @@
         <v>95</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="AA15" s="2" t="s">
         <v>78</v>
@@ -2453,42 +2465,42 @@
         <v>78</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AG15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH15" s="2" t="s">
-        <v>78</v>
-      </c>
     </row>
-    <row r="16" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>45937.248090277775</v>
+        <v>45937.249456018515</v>
       </c>
       <c r="B16" s="1">
-        <v>45937.25240740741</v>
+        <v>45937.25236111111</v>
       </c>
       <c r="C16">
         <v>100</v>
       </c>
       <c r="D16">
-        <v>373</v>
+        <v>250</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F16" s="1">
-        <v>45937.252417337964</v>
+        <v>45937.252370150462</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>66</v>
@@ -2500,37 +2512,37 @@
         <v>68</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>105</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="P16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="T16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="Q16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="U16" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="V16" s="2" t="s">
         <v>73</v>
@@ -2539,60 +2551,60 @@
         <v>88</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="Y16" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AA16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF16" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="AG16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH16" s="2" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>45937.248287037037</v>
+        <v>45937.248090277775</v>
       </c>
       <c r="B17" s="1">
-        <v>45937.252905092595</v>
+        <v>45937.25240740741</v>
       </c>
       <c r="C17">
         <v>100</v>
       </c>
       <c r="D17">
-        <v>399</v>
+        <v>373</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F17" s="1">
-        <v>45937.252912488424</v>
+        <v>45937.252417337964</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>66</v>
@@ -2604,99 +2616,99 @@
         <v>68</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>92</v>
       </c>
       <c r="Q17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="R17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U17" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="V17" s="2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="W17" s="2" t="s">
         <v>88</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="Y17" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z17" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB17" s="2" t="s">
         <v>96</v>
       </c>
       <c r="AC17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AE17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH17" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AF17" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG17" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AH17" s="2" t="s">
-        <v>77</v>
-      </c>
     </row>
-    <row r="18" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>45937.248414351852</v>
+        <v>45937.248287037037</v>
       </c>
       <c r="B18" s="1">
-        <v>45937.252986111111</v>
+        <v>45937.252905092595</v>
       </c>
       <c r="C18">
         <v>100</v>
       </c>
       <c r="D18">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F18" s="1">
-        <v>45937.252994618058</v>
+        <v>45937.252912488424</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>66</v>
@@ -2708,46 +2720,46 @@
         <v>68</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>71</v>
       </c>
       <c r="O18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="P18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P18" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="Q18" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="T18" s="2" t="s">
         <v>72</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="Y18" s="2" t="s">
         <v>95</v>
@@ -2756,51 +2768,51 @@
         <v>77</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AB18" s="2" t="s">
         <v>96</v>
       </c>
       <c r="AC18" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AD18" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AE18" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AF18" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AG18" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AH18" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>45937.250196759262</v>
+        <v>45937.248414351852</v>
       </c>
       <c r="B19" s="1">
-        <v>45937.253333333334</v>
+        <v>45937.252986111111</v>
       </c>
       <c r="C19">
         <v>100</v>
       </c>
       <c r="D19">
-        <v>270</v>
+        <v>394</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F19" s="1">
-        <v>45937.253339201387</v>
+        <v>45937.252994618058</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>66</v>
@@ -2812,13 +2824,13 @@
         <v>68</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>148</v>
+        <v>70</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>71</v>
@@ -2830,7 +2842,7 @@
         <v>86</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="R19" s="2" t="s">
         <v>86</v>
@@ -2842,13 +2854,13 @@
         <v>72</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="V19" s="2" t="s">
         <v>73</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="X19" s="2" t="s">
         <v>94</v>
@@ -2857,19 +2869,19 @@
         <v>95</v>
       </c>
       <c r="Z19" s="2" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB19" s="2" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="AC19" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AE19" s="2" t="s">
         <v>77</v>
@@ -2878,33 +2890,33 @@
         <v>77</v>
       </c>
       <c r="AG19" s="2" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="AH19" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>45937.248124999998</v>
+        <v>45937.250196759262</v>
       </c>
       <c r="B20" s="1">
-        <v>45937.253506944442</v>
+        <v>45937.253333333334</v>
       </c>
       <c r="C20">
         <v>100</v>
       </c>
       <c r="D20">
-        <v>465</v>
+        <v>270</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F20" s="1">
-        <v>45937.253520937498</v>
+        <v>45937.253339201387</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>66</v>
@@ -2916,16 +2928,16 @@
         <v>68</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>152</v>
+        <v>71</v>
       </c>
       <c r="O20" s="2" t="s">
         <v>92</v>
@@ -2937,7 +2949,7 @@
         <v>92</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="S20" s="2" t="s">
         <v>83</v>
@@ -2949,7 +2961,7 @@
         <v>83</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="W20" s="2" t="s">
         <v>74</v>
@@ -2961,10 +2973,10 @@
         <v>95</v>
       </c>
       <c r="Z20" s="2" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="AA20" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AB20" s="2" t="s">
         <v>79</v>
@@ -2973,42 +2985,42 @@
         <v>79</v>
       </c>
       <c r="AD20" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="AE20" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AF20" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AG20" s="2" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="AH20" s="2" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>45937.2496875</v>
+        <v>45937.248124999998</v>
       </c>
       <c r="B21" s="1">
-        <v>45937.253831018519</v>
+        <v>45937.253506944442</v>
       </c>
       <c r="C21">
         <v>100</v>
       </c>
       <c r="D21">
-        <v>357</v>
+        <v>465</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F21" s="1">
-        <v>45937.25383548611</v>
+        <v>45937.253520937498</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>66</v>
@@ -3020,99 +3032,99 @@
         <v>68</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>70</v>
+        <v>151</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="P21" s="2" t="s">
         <v>86</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="T21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="U21" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="V21" s="2" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="Y21" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z21" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AA21" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AB21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AC21" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD21" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AE21" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AF21" s="2" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="AG21" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH21" s="2" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="195" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>45937.250625000001</v>
+        <v>45937.2496875</v>
       </c>
       <c r="B22" s="1">
-        <v>45937.254016203704</v>
+        <v>45937.253831018519</v>
       </c>
       <c r="C22">
         <v>100</v>
       </c>
       <c r="D22">
-        <v>293</v>
+        <v>357</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F22" s="1">
-        <v>45937.254022986112</v>
+        <v>45937.25383548611</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>66</v>
@@ -3124,7 +3136,7 @@
         <v>68</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>82</v>
@@ -3133,52 +3145,52 @@
         <v>70</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q22" s="2" t="s">
         <v>84</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="T22" s="2" t="s">
         <v>83</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="W22" s="2" t="s">
         <v>128</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="Z22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB22" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AA22" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB22" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AC22" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AD22" s="2" t="s">
         <v>77</v>
@@ -3187,36 +3199,36 @@
         <v>77</v>
       </c>
       <c r="AF22" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AG22" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AH22" s="2" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="195" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>45937.249502314815</v>
+        <v>45937.250625000001</v>
       </c>
       <c r="B23" s="1">
-        <v>45937.254363425927</v>
+        <v>45937.254016203704</v>
       </c>
       <c r="C23">
         <v>100</v>
       </c>
       <c r="D23">
-        <v>419</v>
+        <v>293</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F23" s="1">
-        <v>45937.254370590279</v>
+        <v>45937.254022986112</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>66</v>
@@ -3228,64 +3240,64 @@
         <v>68</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>71</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="R23" s="2" t="s">
         <v>85</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="T23" s="2" t="s">
         <v>83</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="Y23" s="2" t="s">
         <v>76</v>
       </c>
       <c r="Z23" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AA23" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AB23" s="2" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="AC23" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AD23" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AE23" s="2" t="s">
         <v>77</v>
@@ -3297,30 +3309,30 @@
         <v>77</v>
       </c>
       <c r="AH23" s="2" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>45937.249756944446</v>
+        <v>45937.249502314815</v>
       </c>
       <c r="B24" s="1">
-        <v>45937.254571759258</v>
+        <v>45937.254363425927</v>
       </c>
       <c r="C24">
         <v>100</v>
       </c>
       <c r="D24">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F24" s="1">
-        <v>45937.254578773151</v>
+        <v>45937.254370590279</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>66</v>
@@ -3332,13 +3344,13 @@
         <v>68</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>71</v>
@@ -3347,49 +3359,49 @@
         <v>83</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q24" s="2" t="s">
         <v>83</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="X24" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="Y24" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="Z24" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AA24" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB24" s="2" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="AC24" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AD24" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AE24" s="2" t="s">
         <v>77</v>
@@ -3401,30 +3413,30 @@
         <v>77</v>
       </c>
       <c r="AH24" s="2" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>45937.2499537037</v>
+        <v>45937.249756944446</v>
       </c>
       <c r="B25" s="1">
-        <v>45937.25613425926</v>
+        <v>45937.254571759258</v>
       </c>
       <c r="C25">
         <v>100</v>
       </c>
       <c r="D25">
-        <v>534</v>
+        <v>415</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F25" s="1">
-        <v>45937.256146608794</v>
+        <v>45937.254578773151</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>66</v>
@@ -3436,95 +3448,187 @@
         <v>68</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>70</v>
+        <v>161</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>71</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q25" s="2" t="s">
         <v>83</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="T25" s="2" t="s">
         <v>72</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="V25" s="2" t="s">
         <v>73</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="Y25" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z25" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA25" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AB25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH25" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" ht="232" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>45937.2499537037</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45937.25613425926</v>
+      </c>
+      <c r="C26">
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>534</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="1">
+        <v>45937.256146608794</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="V26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="X26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB26" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AC25" s="2" t="s">
+      <c r="AC26" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="AD25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH25" s="2" t="s">
+      <c r="AD26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH26" s="2" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AH26" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A3:AH27" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E1:E2 G1:G2 H1:H2 I1:I2 J1:J2 K1:K2 L1:L2 M1:M2 N1:N2 O1:O2 P1:P2 Q1:Q2 R1:R2 S1:S2 T1:T2 U1:U2 V1:V2 W1:W2 X1:X2 Y1:Y2 Z1:Z2 AA1:AA2 AB1:AB2 AC1:AC2 AD1:AD2 AE1:AE2 AF1:AF2 AG1:AG2 AH1:AH2 E3:E25 G3:G25 H3:H25 I3:I25 J3:J25 K3:K25 L3:L25 M3:M25 N3:N25 O3:O25 P3:P25 Q3:Q25 R3:R25 S3:S25 T3:T25 U3:U25 V3:V25 W3:W25 X3:X25 Y3:Y25 Z3:Z25 AA3:AA25 AB3:AB25 AC3:AC25 AD3:AD25 AE3:AE25 AF3:AF25 AG3:AG25 AH3:AH25" numberStoredAsText="1"/>
+    <ignoredError sqref="E2:E3 G2:G3 H2:H3 I2:I3 J2:J3 K2:K3 L2:L3 M2:M3 N2:N3 O2:O3 P2:P3 Q2:Q3 R2:R3 S2:S3 T2:T3 U2:U3 V2:V3 W2:W3 X2:X3 Y2:Y3 Z2:Z3 AA2:AA3 AB2:AB3 AC2:AC3 AD2:AD3 AE2:AE3 AF2:AF3 AG2:AG3 AH2:AH3 E4:E26 G4:G26 H4:H26 I4:I26 J4:J26 K4:K26 L4:L26 M4:M26 N4:N26 O4:O26 P4:P26 Q4:Q26 R4:R26 S4:S26 T4:T26 U4:U26 V4:V26 W4:W26 X4:X26 Y4:Y26 Z4:Z26 AA4:AA26 AB4:AB26 AC4:AC26 AD4:AD26 AE4:AE26 AF4:AF26 AG4:AG26 AH4:AH26" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBBD0717-96DB-49A6-A213-A8BD16C13B46}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Save my local changes
</commit_message>
<xml_diff>
--- a/Datasets/housinggame_session_20_251007_surveys/251009_251007_WhereWeMove sessions - presurvey.xlsx
+++ b/Datasets/housinggame_session_20_251007_surveys/251009_251007_WhereWeMove sessions - presurvey.xlsx
@@ -5,21 +5,33 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/jcortesarevalo_tudelft_nl/Documents/Documents/TUDelft/18_Game Data Analysis/R data analysis BEPs/Datasets/housinggame_session_20_251007_VerzekeraarsMasterClass_surveys/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/jcortesarevalo_tudelft_nl/Documents/Documents/TUDelft/18_Game Data Analysis/R data analysis BEPs/Datasets/housinggame_session_20_251007_surveys/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_F267ED7BEE40FE1B69EAED488EA404700F25161E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94D372DB-EDE7-40AE-B804-5D89E6E43AC8}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_F267ED7BEE40FE1B69EAED488EA404700F25161E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C8D3BA4-1F6E-434F-93BC-B0ABC52D9E03}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet0!$A$2:$AH$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet0!$A$3:$AH$27</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -897,127 +909,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH25"/>
+  <dimension ref="A1:AH26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection sqref="A1:AH1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+      <c r="R1">
+        <v>18</v>
+      </c>
+      <c r="S1">
+        <v>19</v>
+      </c>
+      <c r="T1">
+        <v>20</v>
+      </c>
+      <c r="U1">
+        <v>21</v>
+      </c>
+      <c r="V1">
+        <v>22</v>
+      </c>
+      <c r="W1">
+        <v>23</v>
+      </c>
+      <c r="X1">
+        <v>24</v>
+      </c>
+      <c r="Y1">
+        <v>25</v>
+      </c>
+      <c r="Z1">
+        <v>26</v>
+      </c>
+      <c r="AA1">
+        <v>27</v>
+      </c>
+      <c r="AB1">
+        <v>28</v>
+      </c>
+      <c r="AC1">
+        <v>29</v>
+      </c>
+      <c r="AD1">
+        <v>30</v>
+      </c>
+      <c r="AE1">
+        <v>31</v>
+      </c>
+      <c r="AF1">
+        <v>32</v>
+      </c>
+      <c r="AG1">
+        <v>33</v>
+      </c>
+      <c r="AH1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -1029,218 +1041,218 @@
         <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="195" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="4" spans="1:34" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>45937.245208333334</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>45937.248240740744</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>261</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="1">
-        <v>45937.248254502316</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" ht="240" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>45937.248032407406</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45937.250648148147</v>
       </c>
       <c r="C4">
         <v>100</v>
       </c>
       <c r="D4">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F4" s="1">
-        <v>45937.250662881946</v>
+        <v>45937.248254502316</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>66</v>
@@ -1249,13 +1261,13 @@
         <v>67</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>70</v>
@@ -1264,46 +1276,46 @@
         <v>71</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>85</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>88</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="Z4" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="AC4" s="2" t="s">
         <v>77</v>
@@ -1312,39 +1324,39 @@
         <v>77</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AF4" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="180" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>45937.248437499999</v>
+        <v>45937.248032407406</v>
       </c>
       <c r="B5" s="1">
-        <v>45937.250694444447</v>
+        <v>45937.250648148147</v>
       </c>
       <c r="C5">
         <v>100</v>
       </c>
       <c r="D5">
-        <v>194</v>
+        <v>226</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="1">
-        <v>45937.250705486113</v>
+        <v>45937.250662881946</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>66</v>
@@ -1356,10 +1368,10 @@
         <v>68</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>70</v>
@@ -1368,87 +1380,87 @@
         <v>71</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="S5" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="AC5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AD5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AG5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>78</v>
-      </c>
     </row>
-    <row r="6" spans="1:34" ht="195" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="174" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>45937.24800925926</v>
+        <v>45937.248437499999</v>
       </c>
       <c r="B6" s="1">
-        <v>45937.250706018516</v>
+        <v>45937.250694444447</v>
       </c>
       <c r="C6">
         <v>100</v>
       </c>
       <c r="D6">
-        <v>232</v>
+        <v>194</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F6" s="1">
-        <v>45937.250719328702</v>
+        <v>45937.250705486113</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>66</v>
@@ -1460,61 +1472,61 @@
         <v>68</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AD6" s="2" t="s">
         <v>96</v>
@@ -1523,36 +1535,36 @@
         <v>77</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>45937.248159722221</v>
+        <v>45937.24800925926</v>
       </c>
       <c r="B7" s="1">
-        <v>45937.250810185185</v>
+        <v>45937.250706018516</v>
       </c>
       <c r="C7">
         <v>100</v>
       </c>
       <c r="D7">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F7" s="1">
-        <v>45937.250817812499</v>
+        <v>45937.250719328702</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>66</v>
@@ -1564,55 +1576,55 @@
         <v>68</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="T7" s="2" t="s">
         <v>72</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="V7" s="2" t="s">
         <v>73</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB7" s="2" t="s">
         <v>79</v>
@@ -1630,33 +1642,33 @@
         <v>77</v>
       </c>
       <c r="AG7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH7" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>45937.248622685183</v>
+        <v>45937.248159722221</v>
       </c>
       <c r="B8" s="1">
-        <v>45937.250821759262</v>
+        <v>45937.250810185185</v>
       </c>
       <c r="C8">
         <v>100</v>
       </c>
       <c r="D8">
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F8" s="1">
-        <v>45937.250835729166</v>
+        <v>45937.250817812499</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>66</v>
@@ -1668,99 +1680,99 @@
         <v>68</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="P8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="Q8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="V8" s="2" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="W8" s="2" t="s">
         <v>88</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="Y8" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="AA8" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AB8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD8" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AC8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AE8" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AF8" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AG8" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AH8" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>45937.247939814813</v>
+        <v>45937.248622685183</v>
       </c>
       <c r="B9" s="1">
-        <v>45937.251446759263</v>
+        <v>45937.250821759262</v>
       </c>
       <c r="C9">
         <v>100</v>
       </c>
       <c r="D9">
-        <v>303</v>
+        <v>190</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F9" s="1">
-        <v>45937.251459236111</v>
+        <v>45937.250835729166</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>66</v>
@@ -1772,99 +1784,99 @@
         <v>68</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>85</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="Y9" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA9" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AE9" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AF9" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AG9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH9" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="180" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>45937.248333333337</v>
+        <v>45937.247939814813</v>
       </c>
       <c r="B10" s="1">
-        <v>45937.251562500001</v>
+        <v>45937.251446759263</v>
       </c>
       <c r="C10">
         <v>100</v>
       </c>
       <c r="D10">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F10" s="1">
-        <v>45937.251572372683</v>
+        <v>45937.251459236111</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>66</v>
@@ -1876,99 +1888,99 @@
         <v>68</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>92</v>
       </c>
       <c r="P10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="Q10" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="R10" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AB10" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="AE10" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AH10" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="174" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>45937.247997685183</v>
+        <v>45937.248333333337</v>
       </c>
       <c r="B11" s="1">
-        <v>45937.251967592594</v>
+        <v>45937.251562500001</v>
       </c>
       <c r="C11">
         <v>100</v>
       </c>
       <c r="D11">
-        <v>343</v>
+        <v>279</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F11" s="1">
-        <v>45937.251981296293</v>
+        <v>45937.251572372683</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>66</v>
@@ -1980,64 +1992,64 @@
         <v>68</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>70</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>123</v>
+        <v>71</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="P11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="Q11" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="R11" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="S11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="T11" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="U11" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="W11" s="2" t="s">
         <v>88</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="Z11" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AC11" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="AE11" s="2" t="s">
         <v>77</v>
@@ -2052,27 +2064,27 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>45937.248333333337</v>
+        <v>45937.247997685183</v>
       </c>
       <c r="B12" s="1">
-        <v>45937.252164351848</v>
+        <v>45937.251967592594</v>
       </c>
       <c r="C12">
         <v>100</v>
       </c>
       <c r="D12">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F12" s="1">
-        <v>45937.252174247682</v>
+        <v>45937.251981296293</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>66</v>
@@ -2084,43 +2096,43 @@
         <v>68</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>83</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="U12" s="2" t="s">
         <v>85</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="X12" s="2" t="s">
         <v>124</v>
@@ -2129,10 +2141,10 @@
         <v>95</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AB12" s="2" t="s">
         <v>96</v>
@@ -2141,42 +2153,42 @@
         <v>77</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AE12" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AG12" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>45937.245358796295</v>
+        <v>45937.248333333337</v>
       </c>
       <c r="B13" s="1">
-        <v>45937.252199074072</v>
+        <v>45937.252164351848</v>
       </c>
       <c r="C13">
         <v>100</v>
       </c>
       <c r="D13">
-        <v>590</v>
+        <v>330</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F13" s="1">
-        <v>45937.252205034725</v>
+        <v>45937.252174247682</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>66</v>
@@ -2188,55 +2200,55 @@
         <v>68</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>83</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="U13" s="2" t="s">
         <v>85</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="Y13" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB13" s="2" t="s">
         <v>96</v>
@@ -2245,42 +2257,42 @@
         <v>77</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AE13" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AF13" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AG13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AH13" s="2" t="s">
-        <v>109</v>
-      </c>
     </row>
-    <row r="14" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>45937.249571759261</v>
+        <v>45937.245358796295</v>
       </c>
       <c r="B14" s="1">
-        <v>45937.252314814818</v>
+        <v>45937.252199074072</v>
       </c>
       <c r="C14">
         <v>100</v>
       </c>
       <c r="D14">
-        <v>236</v>
+        <v>590</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F14" s="1">
-        <v>45937.252322499997</v>
+        <v>45937.252205034725</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>66</v>
@@ -2292,22 +2304,22 @@
         <v>68</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>71</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>72</v>
@@ -2316,13 +2328,13 @@
         <v>83</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="T14" s="2" t="s">
         <v>72</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="V14" s="2" t="s">
         <v>73</v>
@@ -2337,54 +2349,54 @@
         <v>95</v>
       </c>
       <c r="Z14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH14" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AA14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG14" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH14" s="2" t="s">
-        <v>79</v>
-      </c>
     </row>
-    <row r="15" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>45937.249456018515</v>
+        <v>45937.249571759261</v>
       </c>
       <c r="B15" s="1">
-        <v>45937.25236111111</v>
+        <v>45937.252314814818</v>
       </c>
       <c r="C15">
         <v>100</v>
       </c>
       <c r="D15">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F15" s="1">
-        <v>45937.252370150462</v>
+        <v>45937.252322499997</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>66</v>
@@ -2396,43 +2408,43 @@
         <v>68</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="O15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="P15" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="S15" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="V15" s="2" t="s">
         <v>73</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="X15" s="2" t="s">
         <v>94</v>
@@ -2441,7 +2453,7 @@
         <v>95</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="AA15" s="2" t="s">
         <v>78</v>
@@ -2453,42 +2465,42 @@
         <v>78</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AG15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH15" s="2" t="s">
-        <v>78</v>
-      </c>
     </row>
-    <row r="16" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>45937.248090277775</v>
+        <v>45937.249456018515</v>
       </c>
       <c r="B16" s="1">
-        <v>45937.25240740741</v>
+        <v>45937.25236111111</v>
       </c>
       <c r="C16">
         <v>100</v>
       </c>
       <c r="D16">
-        <v>373</v>
+        <v>250</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F16" s="1">
-        <v>45937.252417337964</v>
+        <v>45937.252370150462</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>66</v>
@@ -2500,37 +2512,37 @@
         <v>68</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>105</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="P16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="T16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="Q16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="U16" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="V16" s="2" t="s">
         <v>73</v>
@@ -2539,60 +2551,60 @@
         <v>88</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="Y16" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AA16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF16" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="AG16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH16" s="2" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>45937.248287037037</v>
+        <v>45937.248090277775</v>
       </c>
       <c r="B17" s="1">
-        <v>45937.252905092595</v>
+        <v>45937.25240740741</v>
       </c>
       <c r="C17">
         <v>100</v>
       </c>
       <c r="D17">
-        <v>399</v>
+        <v>373</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F17" s="1">
-        <v>45937.252912488424</v>
+        <v>45937.252417337964</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>66</v>
@@ -2604,99 +2616,99 @@
         <v>68</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>92</v>
       </c>
       <c r="Q17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="R17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U17" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="V17" s="2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="W17" s="2" t="s">
         <v>88</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="Y17" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z17" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB17" s="2" t="s">
         <v>96</v>
       </c>
       <c r="AC17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AE17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH17" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AF17" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG17" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AH17" s="2" t="s">
-        <v>77</v>
-      </c>
     </row>
-    <row r="18" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>45937.248414351852</v>
+        <v>45937.248287037037</v>
       </c>
       <c r="B18" s="1">
-        <v>45937.252986111111</v>
+        <v>45937.252905092595</v>
       </c>
       <c r="C18">
         <v>100</v>
       </c>
       <c r="D18">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F18" s="1">
-        <v>45937.252994618058</v>
+        <v>45937.252912488424</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>66</v>
@@ -2708,46 +2720,46 @@
         <v>68</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>71</v>
       </c>
       <c r="O18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="P18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P18" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="Q18" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="T18" s="2" t="s">
         <v>72</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="Y18" s="2" t="s">
         <v>95</v>
@@ -2756,51 +2768,51 @@
         <v>77</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AB18" s="2" t="s">
         <v>96</v>
       </c>
       <c r="AC18" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AD18" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AE18" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AF18" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AG18" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AH18" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>45937.250196759262</v>
+        <v>45937.248414351852</v>
       </c>
       <c r="B19" s="1">
-        <v>45937.253333333334</v>
+        <v>45937.252986111111</v>
       </c>
       <c r="C19">
         <v>100</v>
       </c>
       <c r="D19">
-        <v>270</v>
+        <v>394</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F19" s="1">
-        <v>45937.253339201387</v>
+        <v>45937.252994618058</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>66</v>
@@ -2812,13 +2824,13 @@
         <v>68</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>148</v>
+        <v>70</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>71</v>
@@ -2830,7 +2842,7 @@
         <v>86</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="R19" s="2" t="s">
         <v>86</v>
@@ -2842,13 +2854,13 @@
         <v>72</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="V19" s="2" t="s">
         <v>73</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="X19" s="2" t="s">
         <v>94</v>
@@ -2857,19 +2869,19 @@
         <v>95</v>
       </c>
       <c r="Z19" s="2" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB19" s="2" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="AC19" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AE19" s="2" t="s">
         <v>77</v>
@@ -2878,33 +2890,33 @@
         <v>77</v>
       </c>
       <c r="AG19" s="2" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="AH19" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>45937.248124999998</v>
+        <v>45937.250196759262</v>
       </c>
       <c r="B20" s="1">
-        <v>45937.253506944442</v>
+        <v>45937.253333333334</v>
       </c>
       <c r="C20">
         <v>100</v>
       </c>
       <c r="D20">
-        <v>465</v>
+        <v>270</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F20" s="1">
-        <v>45937.253520937498</v>
+        <v>45937.253339201387</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>66</v>
@@ -2916,16 +2928,16 @@
         <v>68</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>152</v>
+        <v>71</v>
       </c>
       <c r="O20" s="2" t="s">
         <v>92</v>
@@ -2937,7 +2949,7 @@
         <v>92</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="S20" s="2" t="s">
         <v>83</v>
@@ -2949,7 +2961,7 @@
         <v>83</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="W20" s="2" t="s">
         <v>74</v>
@@ -2961,10 +2973,10 @@
         <v>95</v>
       </c>
       <c r="Z20" s="2" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="AA20" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AB20" s="2" t="s">
         <v>79</v>
@@ -2973,42 +2985,42 @@
         <v>79</v>
       </c>
       <c r="AD20" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="AE20" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AF20" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AG20" s="2" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="AH20" s="2" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>45937.2496875</v>
+        <v>45937.248124999998</v>
       </c>
       <c r="B21" s="1">
-        <v>45937.253831018519</v>
+        <v>45937.253506944442</v>
       </c>
       <c r="C21">
         <v>100</v>
       </c>
       <c r="D21">
-        <v>357</v>
+        <v>465</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F21" s="1">
-        <v>45937.25383548611</v>
+        <v>45937.253520937498</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>66</v>
@@ -3020,99 +3032,99 @@
         <v>68</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>70</v>
+        <v>151</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="P21" s="2" t="s">
         <v>86</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="T21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="U21" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="V21" s="2" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="Y21" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z21" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AA21" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AB21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AC21" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD21" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AE21" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AF21" s="2" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="AG21" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH21" s="2" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="195" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>45937.250625000001</v>
+        <v>45937.2496875</v>
       </c>
       <c r="B22" s="1">
-        <v>45937.254016203704</v>
+        <v>45937.253831018519</v>
       </c>
       <c r="C22">
         <v>100</v>
       </c>
       <c r="D22">
-        <v>293</v>
+        <v>357</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F22" s="1">
-        <v>45937.254022986112</v>
+        <v>45937.25383548611</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>66</v>
@@ -3124,7 +3136,7 @@
         <v>68</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>82</v>
@@ -3133,52 +3145,52 @@
         <v>70</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q22" s="2" t="s">
         <v>84</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="T22" s="2" t="s">
         <v>83</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="W22" s="2" t="s">
         <v>128</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="Z22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB22" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AA22" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB22" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AC22" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AD22" s="2" t="s">
         <v>77</v>
@@ -3187,36 +3199,36 @@
         <v>77</v>
       </c>
       <c r="AF22" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AG22" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AH22" s="2" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="195" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>45937.249502314815</v>
+        <v>45937.250625000001</v>
       </c>
       <c r="B23" s="1">
-        <v>45937.254363425927</v>
+        <v>45937.254016203704</v>
       </c>
       <c r="C23">
         <v>100</v>
       </c>
       <c r="D23">
-        <v>419</v>
+        <v>293</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F23" s="1">
-        <v>45937.254370590279</v>
+        <v>45937.254022986112</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>66</v>
@@ -3228,64 +3240,64 @@
         <v>68</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>71</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="R23" s="2" t="s">
         <v>85</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="T23" s="2" t="s">
         <v>83</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="Y23" s="2" t="s">
         <v>76</v>
       </c>
       <c r="Z23" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AA23" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AB23" s="2" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="AC23" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AD23" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AE23" s="2" t="s">
         <v>77</v>
@@ -3297,30 +3309,30 @@
         <v>77</v>
       </c>
       <c r="AH23" s="2" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>45937.249756944446</v>
+        <v>45937.249502314815</v>
       </c>
       <c r="B24" s="1">
-        <v>45937.254571759258</v>
+        <v>45937.254363425927</v>
       </c>
       <c r="C24">
         <v>100</v>
       </c>
       <c r="D24">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F24" s="1">
-        <v>45937.254578773151</v>
+        <v>45937.254370590279</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>66</v>
@@ -3332,13 +3344,13 @@
         <v>68</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>71</v>
@@ -3347,49 +3359,49 @@
         <v>83</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q24" s="2" t="s">
         <v>83</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="X24" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="Y24" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="Z24" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AA24" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB24" s="2" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="AC24" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AD24" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="AE24" s="2" t="s">
         <v>77</v>
@@ -3401,30 +3413,30 @@
         <v>77</v>
       </c>
       <c r="AH24" s="2" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="240" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>45937.2499537037</v>
+        <v>45937.249756944446</v>
       </c>
       <c r="B25" s="1">
-        <v>45937.25613425926</v>
+        <v>45937.254571759258</v>
       </c>
       <c r="C25">
         <v>100</v>
       </c>
       <c r="D25">
-        <v>534</v>
+        <v>415</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F25" s="1">
-        <v>45937.256146608794</v>
+        <v>45937.254578773151</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>66</v>
@@ -3436,95 +3448,187 @@
         <v>68</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>70</v>
+        <v>161</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>71</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q25" s="2" t="s">
         <v>83</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="T25" s="2" t="s">
         <v>72</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="V25" s="2" t="s">
         <v>73</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="Y25" s="2" t="s">
         <v>95</v>
       </c>
       <c r="Z25" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA25" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AB25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH25" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" ht="232" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>45937.2499537037</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45937.25613425926</v>
+      </c>
+      <c r="C26">
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>534</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="1">
+        <v>45937.256146608794</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="V26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="X26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB26" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AC25" s="2" t="s">
+      <c r="AC26" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="AD25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH25" s="2" t="s">
+      <c r="AD26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH26" s="2" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AH26" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A3:AH27" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E1:E2 G1:G2 H1:H2 I1:I2 J1:J2 K1:K2 L1:L2 M1:M2 N1:N2 O1:O2 P1:P2 Q1:Q2 R1:R2 S1:S2 T1:T2 U1:U2 V1:V2 W1:W2 X1:X2 Y1:Y2 Z1:Z2 AA1:AA2 AB1:AB2 AC1:AC2 AD1:AD2 AE1:AE2 AF1:AF2 AG1:AG2 AH1:AH2 E3:E25 G3:G25 H3:H25 I3:I25 J3:J25 K3:K25 L3:L25 M3:M25 N3:N25 O3:O25 P3:P25 Q3:Q25 R3:R25 S3:S25 T3:T25 U3:U25 V3:V25 W3:W25 X3:X25 Y3:Y25 Z3:Z25 AA3:AA25 AB3:AB25 AC3:AC25 AD3:AD25 AE3:AE25 AF3:AF25 AG3:AG25 AH3:AH25" numberStoredAsText="1"/>
+    <ignoredError sqref="E2:E3 G2:G3 H2:H3 I2:I3 J2:J3 K2:K3 L2:L3 M2:M3 N2:N3 O2:O3 P2:P3 Q2:Q3 R2:R3 S2:S3 T2:T3 U2:U3 V2:V3 W2:W3 X2:X3 Y2:Y3 Z2:Z3 AA2:AA3 AB2:AB3 AC2:AC3 AD2:AD3 AE2:AE3 AF2:AF3 AG2:AG3 AH2:AH3 E4:E26 G4:G26 H4:H26 I4:I26 J4:J26 K4:K26 L4:L26 M4:M26 N4:N26 O4:O26 P4:P26 Q4:Q26 R4:R26 S4:S26 T4:T26 U4:U26 V4:V26 W4:W26 X4:X26 Y4:Y26 Z4:Z26 AA4:AA26 AB4:AB26 AC4:AC26 AD4:AD26 AE4:AE26 AF4:AF26 AG4:AG26 AH4:AH26" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBBD0717-96DB-49A6-A213-A8BD16C13B46}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>